<commit_message>
git commit origin main
</commit_message>
<xml_diff>
--- a/Data/Departures_HS_to_Rdam.xlsx
+++ b/Data/Departures_HS_to_Rdam.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\OneDrive\Documenten\TU Delft\1. MSc TIL\Q1\TIL6022\TIL6022_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\PycharmProjects\TIL6022_Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{31DABD19-4837-4BFC-9D95-EBB846FCF556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B60DB2A2-9EDD-479A-89AD-50367475A4AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{6854C589-9831-440A-912D-927872C92CED}"/>
   </bookViews>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
   <si>
     <t>Rdam</t>
   </si>
@@ -57,6 +46,15 @@
   </si>
   <si>
     <t>Schiedam</t>
+  </si>
+  <si>
+    <t>spr</t>
+  </si>
+  <si>
+    <t>IC</t>
+  </si>
+  <si>
+    <t>traintype</t>
   </si>
 </sst>
 </file>
@@ -64,7 +62,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$]hh:mm;@" x16r2:formatCode16="[$-en-NL,1]hh:mm;@"/>
+    <numFmt numFmtId="164" formatCode="[$]hh:mm;@" x16r2:formatCode16="[$-en-NL,1]hh:mm;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -97,7 +95,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -412,15 +410,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{400D6DDE-974E-45AF-A3CA-7924D6FD2321}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -442,8 +440,11 @@
       <c r="G1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1">
         <v>0.67291666666666661</v>
       </c>
@@ -465,8 +466,11 @@
       <c r="G2" s="1">
         <v>0.68958333333333333</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>0.67986111111111114</v>
       </c>
@@ -482,8 +486,11 @@
       <c r="G3" s="1">
         <v>0.69305555555555554</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <v>0.68263888888888891</v>
       </c>
@@ -497,8 +504,11 @@
       <c r="G4" s="1">
         <v>0.69513888888888886</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>0.68680555555555556</v>
       </c>
@@ -514,8 +524,11 @@
       <c r="G5" s="1">
         <v>0.70000000000000007</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
         <v>0.69374999999999998</v>
       </c>
@@ -537,8 +550,11 @@
       <c r="G6" s="1">
         <v>0.7104166666666667</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
         <v>0.7006944444444444</v>
       </c>
@@ -554,8 +570,11 @@
       <c r="G7" s="1">
         <v>0.71388888888888891</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
         <v>0.70347222222222217</v>
       </c>
@@ -569,8 +588,11 @@
       <c r="G8" s="1">
         <v>0.71597222222222223</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1">
         <v>0.70763888888888893</v>
       </c>
@@ -586,8 +608,11 @@
       <c r="G9" s="1">
         <v>0.72083333333333333</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1">
         <v>0.71458333333333324</v>
       </c>
@@ -609,8 +634,11 @@
       <c r="G10" s="1">
         <v>0.73125000000000007</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1">
         <v>0.72152777777777777</v>
       </c>
@@ -626,8 +654,11 @@
       <c r="G11" s="1">
         <v>0.73472222222222217</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1">
         <v>0.72430555555555554</v>
       </c>
@@ -641,8 +672,11 @@
       <c r="G12" s="1">
         <v>0.7368055555555556</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1">
         <v>0.7284722222222223</v>
       </c>
@@ -658,8 +692,11 @@
       <c r="G13" s="1">
         <v>0.7416666666666667</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1">
         <v>0.73541666666666661</v>
       </c>
@@ -681,8 +718,11 @@
       <c r="G14" s="1">
         <v>0.75208333333333333</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1">
         <v>0.74236111111111114</v>
       </c>
@@ -698,8 +738,11 @@
       <c r="G15" s="1">
         <v>0.75555555555555554</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1">
         <v>0.74513888888888891</v>
       </c>
@@ -713,8 +756,11 @@
       <c r="G16" s="1">
         <v>0.75763888888888886</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1">
         <v>0.74930555555555556</v>
       </c>
@@ -730,8 +776,11 @@
       <c r="G17" s="1">
         <v>0.76250000000000007</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -740,7 +789,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -749,7 +798,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -758,7 +807,7 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -767,7 +816,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -776,7 +825,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -785,7 +834,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -794,7 +843,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>

</xml_diff>